<commit_message>
fix import authentication error!
</commit_message>
<xml_diff>
--- a/excel/s_buff.xlsx
+++ b/excel/s_buff.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
-    <sheet name="buff" sheetId="1" r:id="rId1"/>
+    <sheet name="buffConfig" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -2036,7 +2036,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
   <si>
     <t>状态ID</t>
   </si>
@@ -2241,6 +2241,70 @@
   </si>
   <si>
     <t>AttributionType:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttributionType:11;ValueType:0;Value:200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9,0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttributionType:30;ValueType:1;Value:100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttributionType:7;ValueType:0;Value:1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttributionType:40;ValueType:1;Value:150</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>AttributionType:39;ValueType:2;Value:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>AttributionType:12;ValueType:0;Value:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-1000</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttributionType:39;ValueType:2;Value:8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttributionType:8;ValueType:0;Value:-100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttributionType:32;ValueType:2;Value:12</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2248,7 +2312,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2291,6 +2355,20 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2616,10 +2694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4275,6 +4353,386 @@
         <v>0</v>
       </c>
     </row>
+    <row r="44" spans="1:12">
+      <c r="A44">
+        <v>66</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>66</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>150</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44" t="s">
+        <v>59</v>
+      </c>
+      <c r="L44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45">
+        <v>67</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>67</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45" t="b">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>90</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>4</v>
+      </c>
+      <c r="K45" t="s">
+        <v>40</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46">
+        <v>68</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>68</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46" t="s">
+        <v>61</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47">
+        <v>69</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>69</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47" t="s">
+        <v>62</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48">
+        <v>70</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>70</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48" t="s">
+        <v>68</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49">
+        <v>71</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>71</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" t="b">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>150</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49" t="s">
+        <v>63</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50">
+        <v>72</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>72</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50" t="s">
+        <v>64</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51">
+        <v>73</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>73</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" t="b">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>150</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51" t="s">
+        <v>65</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52">
+        <v>74</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>74</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" t="b">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>90</v>
+      </c>
+      <c r="H52">
+        <v>90</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52" t="s">
+        <v>66</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53">
+        <v>75</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>75</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53" t="s">
+        <v>67</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>